<commit_message>
Registro: Modificar almacenamiento de datos
* Elimina columna "A CUENTA", ya que es obsoleto.
* Ajusta a un nuevo tamaño el contenido de las celdas.
* Cambia TIPO DE PAGO por CONCEPTO al aceptar dos métodos de pago.
* Cambios estéticos.

Signed-off-by: qaotyk <mayniakgd@gmail.com>
</commit_message>
<xml_diff>
--- a/registro_main.xlsx
+++ b/registro_main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QAOTYK\Desktop\registro_excel_macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C3149E-1553-4644-946C-FFF94D3B3B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F45E84-A6CC-4453-8D3A-F3DFC3B840D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3AF314D-D49C-4E56-878F-BFC4E127C6E3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>FECHA</t>
   </si>
@@ -54,25 +54,28 @@
     <t>TELEFONO</t>
   </si>
   <si>
-    <t>TIPO DE PAGO</t>
-  </si>
-  <si>
-    <t>A CUENTA</t>
-  </si>
-  <si>
     <t>EFECTIVO</t>
   </si>
   <si>
     <t>TARJETA</t>
   </si>
   <si>
-    <t>TOTAL DE VENTA</t>
-  </si>
-  <si>
     <t>CIERRE/DIA</t>
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>CONCEPTO</t>
+  </si>
+  <si>
+    <t>FORMA DE PAGO</t>
+  </si>
+  <si>
+    <t>VENTA</t>
+  </si>
+  <si>
+    <t>TOTAL DE</t>
   </si>
 </sst>
 </file>
@@ -169,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -239,7 +242,31 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -249,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -276,9 +303,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -304,16 +328,46 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -631,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047E54BC-2388-4289-9894-A5CEAA9ACA7E}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,29 +697,39 @@
     <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.42578125" style="4"/>
+    <col min="8" max="10" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="19"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="str">
+    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="str">
         <f>UPPER(TEXT(A4,"DDDD"))</f>
         <v>SÁBADO</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="H2" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -680,336 +744,309 @@
       <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="18" t="str">
+      <c r="B24" s="17" t="str">
         <f>SUM(B4:B23)&amp;" Artículos"</f>
         <v>0 Artículos</v>
       </c>
@@ -1018,29 +1055,33 @@
       <c r="E24" s="6"/>
       <c r="F24" s="7"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="12">
+      <c r="H24" s="11">
+        <f>SUM(H4:H23)</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="11">
         <f>SUM(I4:I23)</f>
         <v>0</v>
       </c>
-      <c r="J24" s="12">
+      <c r="J24" s="11">
+        <f>SUM(H24:I24)</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="11">
         <f>SUM(J4:J23)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="12">
-        <f>SUM(I24:J24)</f>
+      <c r="L24" s="10">
+        <f>SUM(K24)</f>
         <v>0</v>
       </c>
-      <c r="L24" s="12">
-        <f>SUM(K4:K23)</f>
-        <v>0</v>
-      </c>
-      <c r="M24" s="11">
-        <f>SUM(L24)</f>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Registro: Inmovilizar fila superior
* Mantiene visible la fila superior a medida que se desplaza
  por el resto de la hoja de cálculo.

Signed-off-by: qaotyk <mayniakgd@gmail.com>
</commit_message>
<xml_diff>
--- a/registro_main.xlsx
+++ b/registro_main.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QAOTYK\Desktop\registro_excel_macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F45E84-A6CC-4453-8D3A-F3DFC3B840D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DCA482-2BD9-4BA5-B1D8-B2F50044241A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3AF314D-D49C-4E56-878F-BFC4E127C6E3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="REPORTE" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>FECHA</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>TOTAL DE</t>
+  </si>
+  <si>
+    <t>TOTAL DE VENTA</t>
   </si>
 </sst>
 </file>
@@ -276,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -364,10 +367,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -685,10 +694,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047E54BC-2388-4289-9894-A5CEAA9ACA7E}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,95 +710,120 @@
     <col min="5" max="5" width="25.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.140625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="18"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="str">
-        <f>UPPER(TEXT(A4,"DDDD"))</f>
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="str">
+        <f>UPPER(TEXT(A5,"DDDD"))</f>
         <v>SÁBADO</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="31" t="s">
+      <c r="I3" s="31"/>
+      <c r="J3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K3" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L3" s="32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J4" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="7"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="25"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
@@ -1042,45 +1077,59 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="17" t="str">
-        <f>SUM(B4:B23)&amp;" Artículos"</f>
+      <c r="B25" s="17" t="str">
+        <f>SUM(B5:B24)&amp;" Artículos"</f>
         <v>0 Artículos</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="11">
-        <f>SUM(H4:H23)</f>
+      <c r="C25" s="6"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="11">
+        <f>SUM(H5:H24)</f>
         <v>0</v>
       </c>
-      <c r="I24" s="11">
-        <f>SUM(I4:I23)</f>
+      <c r="I25" s="11">
+        <f>SUM(I5:I24)</f>
         <v>0</v>
       </c>
-      <c r="J24" s="11">
-        <f>SUM(H24:I24)</f>
+      <c r="J25" s="11">
+        <f>SUM(H25:I25)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="11">
-        <f>SUM(J4:J23)</f>
+      <c r="K25" s="11">
+        <f>SUM(J5:J24)</f>
         <v>0</v>
       </c>
-      <c r="L24" s="10">
-        <f>SUM(K24)</f>
+      <c r="L25" s="10">
+        <f>SUM(K25)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>